<commit_message>
feat: add TL-BMF for diet and species
</commit_message>
<xml_diff>
--- a/inst/results/BMF_computation_PCB_ng_glw/1.BMF_species_PCB_ng_glw_summarised.xlsx
+++ b/inst/results/BMF_computation_PCB_ng_glw/1.BMF_species_PCB_ng_glw_summarised.xlsx
@@ -386,13 +386,13 @@
         </is>
       </c>
       <c r="B2">
-        <v>0.8100000000000001</v>
+        <v>0.77</v>
       </c>
       <c r="C2">
-        <v>1.22</v>
+        <v>1.05</v>
       </c>
       <c r="D2">
-        <v>1.62</v>
+        <v>1.15</v>
       </c>
     </row>
     <row r="3">
@@ -402,13 +402,13 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.38</v>
+        <v>0.37</v>
       </c>
       <c r="C3">
-        <v>0.6</v>
+        <v>0.63</v>
       </c>
       <c r="D3">
-        <v>1.02</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="4">
@@ -418,13 +418,13 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.14</v>
+        <v>0.12</v>
       </c>
       <c r="C4">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
       <c r="D4">
-        <v>0.76</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="5">
@@ -434,13 +434,13 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.58</v>
+        <v>0.54</v>
       </c>
       <c r="C5">
-        <v>0.92</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="D5">
-        <v>1.64</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="6">
@@ -450,13 +450,13 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.57</v>
+        <v>0.54</v>
       </c>
       <c r="C6">
-        <v>1.03</v>
+        <v>0.98</v>
       </c>
       <c r="D6">
-        <v>1.65</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="7">
@@ -466,13 +466,13 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.68</v>
+        <v>0.63</v>
       </c>
       <c r="C7">
-        <v>1.22</v>
+        <v>1.21</v>
       </c>
       <c r="D7">
-        <v>1.76</v>
+        <v>1.63</v>
       </c>
     </row>
     <row r="8">
@@ -482,13 +482,13 @@
         </is>
       </c>
       <c r="B8">
-        <v>1.23</v>
+        <v>0.73</v>
       </c>
       <c r="C8">
-        <v>1.9</v>
+        <v>1.02</v>
       </c>
       <c r="D8">
-        <v>2.58</v>
+        <v>1.41</v>
       </c>
     </row>
     <row r="9">
@@ -498,13 +498,13 @@
         </is>
       </c>
       <c r="B9">
-        <v>0.7</v>
+        <v>0.66</v>
       </c>
       <c r="C9">
-        <v>1.36</v>
+        <v>0.99</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>1.34</v>
       </c>
     </row>
     <row r="10">
@@ -514,13 +514,13 @@
         </is>
       </c>
       <c r="B10">
-        <v>1.29</v>
+        <v>0.65</v>
       </c>
       <c r="C10">
-        <v>1.86</v>
+        <v>0.89</v>
       </c>
       <c r="D10">
-        <v>2.57</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="11">
@@ -530,13 +530,13 @@
         </is>
       </c>
       <c r="B11">
-        <v>0.88</v>
+        <v>0.87</v>
       </c>
       <c r="C11">
-        <v>1.35</v>
+        <v>1.16</v>
       </c>
       <c r="D11">
-        <v>1.97</v>
+        <v>1.52</v>
       </c>
     </row>
     <row r="12">
@@ -546,13 +546,13 @@
         </is>
       </c>
       <c r="B12">
-        <v>1.34</v>
+        <v>0.72</v>
       </c>
       <c r="C12">
-        <v>2.34</v>
+        <v>0.95</v>
       </c>
       <c r="D12">
-        <v>2.94</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="13">
@@ -562,13 +562,13 @@
         </is>
       </c>
       <c r="B13">
-        <v>0.86</v>
+        <v>0.5</v>
       </c>
       <c r="C13">
-        <v>1.33</v>
+        <v>0.68</v>
       </c>
       <c r="D13">
-        <v>1.87</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="14">
@@ -578,13 +578,13 @@
         </is>
       </c>
       <c r="B14">
-        <v>0.82</v>
+        <v>0.79</v>
       </c>
       <c r="C14">
-        <v>1.29</v>
+        <v>1.03</v>
       </c>
       <c r="D14">
-        <v>2.09</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="15">
@@ -594,13 +594,13 @@
         </is>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0.65</v>
       </c>
       <c r="C15">
-        <v>1.34</v>
+        <v>0.77</v>
       </c>
       <c r="D15">
-        <v>1.83</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="16">
@@ -610,13 +610,13 @@
         </is>
       </c>
       <c r="B16">
-        <v>1.02</v>
+        <v>0.83</v>
       </c>
       <c r="C16">
-        <v>1.41</v>
+        <v>1.1</v>
       </c>
       <c r="D16">
-        <v>1.89</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="17">
@@ -626,13 +626,13 @@
         </is>
       </c>
       <c r="B17">
-        <v>0.6899999999999999</v>
+        <v>0.72</v>
       </c>
       <c r="C17">
-        <v>1.02</v>
+        <v>1.04</v>
       </c>
       <c r="D17">
-        <v>1.29</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="18">
@@ -642,13 +642,13 @@
         </is>
       </c>
       <c r="B18">
-        <v>0.85</v>
+        <v>0.72</v>
       </c>
       <c r="C18">
-        <v>1.16</v>
+        <v>1.11</v>
       </c>
       <c r="D18">
-        <v>1.71</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="19">
@@ -658,13 +658,13 @@
         </is>
       </c>
       <c r="B19">
-        <v>0.98</v>
+        <v>0.75</v>
       </c>
       <c r="C19">
-        <v>1.62</v>
+        <v>1.16</v>
       </c>
       <c r="D19">
-        <v>2.24</v>
+        <v>1.71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remise à niveau git
</commit_message>
<xml_diff>
--- a/inst/results/BMF_computation_PCB_ng_glw/1.BMF_species_PCB_ng_glw_summarised.xlsx
+++ b/inst/results/BMF_computation_PCB_ng_glw/1.BMF_species_PCB_ng_glw_summarised.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -667,6 +667,38 @@
         <v>1.71</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>CB187</t>
+        </is>
+      </c>
+      <c r="B20">
+        <v>0.73</v>
+      </c>
+      <c r="C20">
+        <v>0.93</v>
+      </c>
+      <c r="D20">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>CB194</t>
+        </is>
+      </c>
+      <c r="B21">
+        <v>0.57</v>
+      </c>
+      <c r="C21">
+        <v>0.77</v>
+      </c>
+      <c r="D21">
+        <v>1.14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>